<commit_message>
edit form Import Labour to Add column excel labour_visa_run_date Add file addressID.xls
</commit_message>
<xml_diff>
--- a/public/master-import-file/address.xlsx
+++ b/public/master-import-file/address.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC-TFG091.THEFIRSTGOOD\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\labour-edition\public\master-import-file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8902D083-80B3-4BB1-A7D3-9B3863E9320B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC4D5E51-E692-474C-BF5C-BA15F5818827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -424,8 +424,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -435,8 +435,9 @@
     <col min="3" max="3" width="23.5703125" style="3" customWidth="1"/>
     <col min="4" max="4" width="22.28515625" style="3" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="43.85546875" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="2"/>
+    <col min="6" max="6" width="34.5703125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" style="2" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="23.25" x14ac:dyDescent="0.5">

</xml_diff>